<commit_message>
personal form bug fixed
</commit_message>
<xml_diff>
--- a/assets/ex.xlsx
+++ b/assets/ex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\flutter_vscode\Diet\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\proj\Diet\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60F1ED3-3C53-4008-8396-F1FEE5E12A8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87DBEC1-5F24-4FEB-8838-1A9BFE021155}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17010" yWindow="1890" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="원본" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>D000006</t>
   </si>
@@ -61,9 +61,6 @@
     <t>D000022</t>
   </si>
   <si>
-    <t>D000023</t>
-  </si>
-  <si>
     <t>음식</t>
   </si>
   <si>
@@ -101,9 +98,6 @@
   </si>
   <si>
     <t>양념장어구이</t>
-  </si>
-  <si>
-    <t>임연수구이</t>
   </si>
   <si>
     <t>구이류</t>
@@ -180,7 +174,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -521,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R11" sqref="Q11:R11"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -539,369 +533,388 @@
     <col min="8" max="8" width="12.75" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="3">
+        <v>26</v>
+      </c>
+      <c r="E1">
         <v>0.73760000000000003</v>
       </c>
-      <c r="F1" s="3">
+      <c r="F1">
+        <v>7.9400000000000012E-2</v>
+      </c>
+      <c r="G1">
         <v>6.7000000000000004E-2</v>
       </c>
-      <c r="G1" s="3">
+      <c r="H1">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="H1" s="3">
-        <v>7.9400000000000012E-2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="3">
+        <v>26</v>
+      </c>
+      <c r="E2">
         <v>1.489025</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2">
+        <v>0.11225</v>
+      </c>
+      <c r="G2">
         <v>0.11474999999999999</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2">
         <v>6.4500000000000002E-2</v>
       </c>
-      <c r="H2" s="3">
-        <v>0.11225</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="3">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="3">
+        <v>26</v>
+      </c>
+      <c r="E3">
         <v>1.8615666666666668</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="G3">
         <v>0.15166666666666667</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3">
         <v>0.10533333333333333</v>
       </c>
-      <c r="H3" s="3">
-        <v>7.6999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="3">
+        <v>26</v>
+      </c>
+      <c r="E4">
         <v>2.5246142857142857</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
+        <v>0.19068571428571429</v>
+      </c>
+      <c r="G4">
         <v>0.16517142857142855</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4">
         <v>0.12235714285714284</v>
       </c>
-      <c r="H4" s="3">
-        <v>0.19068571428571429</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="3">
+        <v>26</v>
+      </c>
+      <c r="E5">
         <v>1.84</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
+        <v>0.311</v>
+      </c>
+      <c r="G5">
         <v>3.1E-2</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5">
         <v>5.2000000000000005E-2</v>
       </c>
-      <c r="H5" s="3">
-        <v>0.311</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" s="3">
+        <v>26</v>
+      </c>
+      <c r="E6">
         <v>1.5880000000000001</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
+        <v>8.4000000000000012E-3</v>
+      </c>
+      <c r="G6">
         <v>0.24440000000000001</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6">
         <v>6.6000000000000003E-2</v>
       </c>
-      <c r="H6" s="3">
-        <v>8.4000000000000012E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="3">
+        <v>26</v>
+      </c>
+      <c r="E7">
         <v>2.4032</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="G7">
         <v>0.19500000000000001</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7">
         <v>0.14400000000000002</v>
       </c>
-      <c r="H7" s="3">
-        <v>8.1000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="3">
+        <v>26</v>
+      </c>
+      <c r="E8">
         <v>1.952</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="G8">
         <v>0.21840000000000001</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8">
         <v>0.1232</v>
       </c>
-      <c r="H8" s="3">
-        <v>8.0000000000000004E-4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="3">
+        <v>26</v>
+      </c>
+      <c r="E9">
         <v>2.6352666666666669</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G9">
         <v>0.22933333333333333</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9">
         <v>0.16799999999999998</v>
       </c>
-      <c r="H9" s="3">
-        <v>5.1999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="3">
+        <v>26</v>
+      </c>
+      <c r="E10">
         <v>2.9654000000000003</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
+        <v>0.11599999999999999</v>
+      </c>
+      <c r="G10">
         <v>0.26</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10">
         <v>0.16200000000000001</v>
       </c>
-      <c r="H10" s="3">
-        <v>0.11599999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I10" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="3">
+        <v>26</v>
+      </c>
+      <c r="E11">
         <v>3.2971666666666666</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
+        <v>8.7333333333333332E-2</v>
+      </c>
+      <c r="G11">
         <v>0.20033333333333334</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11">
         <v>0.23866666666666664</v>
       </c>
-      <c r="H11" s="3">
-        <v>8.7333333333333332E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I11" s="3">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="3">
+        <v>26</v>
+      </c>
+      <c r="E12">
         <v>3.2054</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
+        <v>9.1333333333333322E-2</v>
+      </c>
+      <c r="G12">
         <v>0.18066666666666667</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12">
         <v>0.23533333333333331</v>
       </c>
-      <c r="H12" s="3">
-        <v>9.1333333333333322E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I12" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="3">
+        <v>26</v>
+      </c>
+      <c r="E13">
         <v>2.8890133333333332</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
+        <v>5.8693333333333333E-2</v>
+      </c>
+      <c r="G13">
         <v>0.20514000000000002</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13">
         <v>0.20374</v>
       </c>
-      <c r="H13" s="3">
-        <v>5.8693333333333333E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="3">
-        <v>1.976</v>
-      </c>
-      <c r="F14" s="3">
-        <v>0.2152</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.1176</v>
-      </c>
-      <c r="H14" s="3">
-        <v>1.4E-2</v>
-      </c>
+      <c r="I13" s="3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>